<commit_message>
added the binding object that was missing.
</commit_message>
<xml_diff>
--- a/docs/Estimation.xlsx
+++ b/docs/Estimation.xlsx
@@ -4,17 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18732" windowHeight="5760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162912"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Module Name</t>
   </si>
@@ -59,13 +63,16 @@
   </si>
   <si>
     <t>Take Assessment</t>
+  </si>
+  <si>
+    <t>2 hrs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,8 +123,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -394,14 +429,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.26171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.41796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.3671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -422,7 +462,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -435,7 +475,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -446,7 +486,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -455,20 +495,22 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -477,7 +519,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -490,7 +532,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -499,7 +541,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>